<commit_message>
Added math formula for band Fc and Q calculations
</commit_message>
<xml_diff>
--- a/bands.xlsx
+++ b/bands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcobrattinga/GITREPO/vocoder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B527A387-2CDE-D646-A277-F14C801D805E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCFCB37-DD7A-264D-832D-D401553719C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16560" activeTab="1" xr2:uid="{9AF15C12-F13F-DD40-AB91-250BCFB6CE6C}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16540" activeTab="1" xr2:uid="{9AF15C12-F13F-DD40-AB91-250BCFB6CE6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Bands" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="162">
   <si>
     <t>Note</t>
   </si>
@@ -516,6 +516,12 @@
   </si>
   <si>
     <t>910k</t>
+  </si>
+  <si>
+    <t>Sallen-Key low pass</t>
+  </si>
+  <si>
+    <t>Sallen-Key high pass</t>
   </si>
 </sst>
 </file>
@@ -889,7 +895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE833422-419B-2F49-948A-0FCADFD469A4}">
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
@@ -3247,7 +3253,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3320,15 +3326,15 @@
         <v>2000</v>
       </c>
       <c r="E3">
-        <v>120000</v>
+        <v>200000</v>
       </c>
       <c r="F3">
         <f>1/(2*PI()*SQRT(A3*$B$1*$B$1*B3*E3*(C3*D3/(C3+D3))))</f>
-        <v>155.59034733832456</v>
+        <v>120.51976481439172</v>
       </c>
       <c r="G3">
         <f>E3/(2*SQRT(E3*(C3*D3/(C3+D3))))</f>
-        <v>3.9886201760873279</v>
+        <v>5.1492865054443726</v>
       </c>
       <c r="K3" t="s">
         <v>88</v>
@@ -3358,6 +3364,9 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>160</v>
+      </c>
       <c r="K5" t="s">
         <v>90</v>
       </c>
@@ -3372,6 +3381,24 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>83</v>
+      </c>
       <c r="K6" t="s">
         <v>91</v>
       </c>
@@ -3386,6 +3413,26 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="B7">
+        <v>68</v>
+      </c>
+      <c r="C7">
+        <v>150000</v>
+      </c>
+      <c r="D7">
+        <v>150000</v>
+      </c>
+      <c r="F7">
+        <f>1/(2*PI()*SQRT(C7*$B$1*A7*$B$1*D7*B7))</f>
+        <v>171.94137788983227</v>
+      </c>
+      <c r="G7">
+        <f>SQRT(B7/A7)/2</f>
+        <v>5.5097316501933973</v>
+      </c>
       <c r="K7" t="s">
         <v>92</v>
       </c>
@@ -3414,6 +3461,9 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>161</v>
+      </c>
       <c r="K9" t="s">
         <v>94</v>
       </c>
@@ -3428,6 +3478,24 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>83</v>
+      </c>
       <c r="K10" t="s">
         <v>95</v>
       </c>
@@ -3442,6 +3510,26 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>3300</v>
+      </c>
+      <c r="D11">
+        <v>150000</v>
+      </c>
+      <c r="F11">
+        <f>1/(2*PI()*SQRT(C11*$B$1*A11*$B$1*D11*B11))</f>
+        <v>7153.4827161933972</v>
+      </c>
+      <c r="G11">
+        <f>SQRT(D11/C11)/2</f>
+        <v>3.3709993123162105</v>
+      </c>
       <c r="K11" t="s">
         <v>96</v>
       </c>

</xml_diff>